<commit_message>
some changes on estimates
</commit_message>
<xml_diff>
--- a/ofc/estimates/Baniyaa gaun/chinimaya mam ghar paxadi.xlsx
+++ b/ofc/estimates/Baniyaa gaun/chinimaya mam ghar paxadi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.Estimate" sheetId="15" r:id="rId1"/>
@@ -37,12 +37,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">WCR!$A$1:$K$32</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -213,15 +213,18 @@
   </si>
   <si>
     <t>-for empty bag filling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project:- मनोहरा नदि कटानबाट पहिरो संरक्षण कार्य </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -424,21 +427,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -453,7 +456,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,7 +506,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,7 +520,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,7 +532,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -542,7 +545,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -562,7 +565,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -627,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1288,21 +1291,21 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +1320,7 @@
       <c r="J1" s="63"/>
       <c r="K1" s="63"/>
     </row>
-    <row r="2" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>1</v>
       </c>
@@ -1332,7 +1335,7 @@
       <c r="J2" s="64"/>
       <c r="K2" s="64"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
@@ -1347,7 +1350,7 @@
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
@@ -1362,7 +1365,7 @@
       <c r="J4" s="65"/>
       <c r="K4" s="65"/>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>4</v>
       </c>
@@ -1377,7 +1380,7 @@
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
         <v>54</v>
       </c>
@@ -1394,7 +1397,7 @@
       <c r="J6" s="62"/>
       <c r="K6" s="62"/>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>6</v>
       </c>
@@ -1411,7 +1414,7 @@
       <c r="J7" s="69"/>
       <c r="K7" s="69"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -1463,7 +1466,7 @@
       <c r="J9" s="15"/>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="17">
@@ -1487,7 +1490,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
         <v>18</v>
@@ -1512,7 +1515,7 @@
       </c>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
@@ -1525,7 +1528,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>2</v>
       </c>
@@ -1542,7 +1545,7 @@
       <c r="J13" s="15"/>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10">
@@ -1570,7 +1573,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9" t="s">
         <v>18</v>
@@ -1595,7 +1598,7 @@
       </c>
       <c r="K15" s="72"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -1608,7 +1611,7 @@
       <c r="J16" s="15"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>3</v>
       </c>
@@ -1625,7 +1628,7 @@
       <c r="J17" s="15"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>47</v>
@@ -1648,7 +1651,7 @@
       <c r="J18" s="20"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
         <v>48</v>
@@ -1671,7 +1674,7 @@
       <c r="J19" s="20"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
         <v>18</v>
@@ -1696,7 +1699,7 @@
       </c>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
         <v>20</v>
@@ -1714,7 +1717,7 @@
       </c>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -1727,7 +1730,7 @@
       <c r="J22" s="15"/>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>4</v>
       </c>
@@ -1756,7 +1759,7 @@
       </c>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -1769,7 +1772,7 @@
       <c r="J24" s="15"/>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5</v>
       </c>
@@ -1798,7 +1801,7 @@
       </c>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="24"/>
       <c r="C26" s="10"/>
@@ -1811,7 +1814,7 @@
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="35" t="s">
         <v>29</v>
@@ -1829,7 +1832,7 @@
       </c>
       <c r="K27" s="17"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="53"/>
       <c r="B28" s="54"/>
       <c r="C28" s="55"/>
@@ -1842,7 +1845,7 @@
       <c r="J28" s="57"/>
       <c r="K28" s="58"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="22" t="s">
         <v>23</v>
@@ -1862,7 +1865,7 @@
       <c r="J29" s="30"/>
       <c r="K29" s="31"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="32"/>
       <c r="B30" s="22" t="s">
         <v>24</v>
@@ -1879,7 +1882,7 @@
       <c r="J30" s="34"/>
       <c r="K30" s="33"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
       <c r="B31" s="22" t="s">
         <v>25</v>
@@ -1900,7 +1903,7 @@
       <c r="J31" s="34"/>
       <c r="K31" s="33"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="32"/>
       <c r="B32" s="22" t="s">
         <v>26</v>
@@ -1921,7 +1924,7 @@
       <c r="J32" s="34"/>
       <c r="K32" s="33"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="22" t="s">
         <v>27</v>
@@ -1941,7 +1944,7 @@
       <c r="J33" s="34"/>
       <c r="K33" s="33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
       <c r="B34" s="22" t="s">
         <v>28</v>
@@ -1999,23 +2002,23 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
@@ -2030,7 +2033,7 @@
       <c r="J1" s="82"/>
       <c r="K1" s="82"/>
     </row>
-    <row r="2" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A2" s="83" t="s">
         <v>1</v>
       </c>
@@ -2045,7 +2048,7 @@
       <c r="J2" s="83"/>
       <c r="K2" s="83"/>
     </row>
-    <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
@@ -2060,7 +2063,7 @@
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
     </row>
-    <row r="4" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
@@ -2075,7 +2078,7 @@
       <c r="J4" s="65"/>
       <c r="K4" s="65"/>
     </row>
-    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="84" t="s">
         <v>30</v>
       </c>
@@ -2090,7 +2093,7 @@
       <c r="J5" s="84"/>
       <c r="K5" s="84"/>
     </row>
-    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>31</v>
       </c>
@@ -2113,7 +2116,7 @@
       </c>
       <c r="K6" s="81"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>33</v>
       </c>
@@ -2128,7 +2131,7 @@
       <c r="J7" s="77"/>
       <c r="K7" s="77"/>
     </row>
-    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="61" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -2144,7 +2147,7 @@
       <c r="J8" s="78"/>
       <c r="K8" s="78"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -2160,7 +2163,7 @@
       <c r="J9" s="78"/>
       <c r="K9" s="78"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
         <v>35</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="74"/>
       <c r="B12" s="74"/>
       <c r="C12" s="74"/>
@@ -2212,7 +2215,7 @@
       <c r="J12" s="74"/>
       <c r="K12" s="73"/>
     </row>
-    <row r="13" spans="1:13" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49" t="e">
         <f>'1.Estimate'!#REF!</f>
         <v>#REF!</v>
@@ -2259,7 +2262,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="22"/>
       <c r="C14" s="41"/>
@@ -2273,7 +2276,7 @@
       <c r="K14" s="43"/>
       <c r="M14" s="52"/>
     </row>
-    <row r="15" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="49">
         <f>'1.Estimate'!A9</f>
         <v>1</v>
@@ -2320,7 +2323,7 @@
         <v>10198.391249999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="22"/>
       <c r="C16" s="41"/>
@@ -2334,7 +2337,7 @@
       <c r="K16" s="43"/>
       <c r="M16" s="52"/>
     </row>
-    <row r="17" spans="1:13" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="49">
         <f>'1.Estimate'!A13</f>
         <v>2</v>
@@ -2381,7 +2384,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="48" t="e">
         <f>'1.Estimate'!#REF!</f>
@@ -2410,7 +2413,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="22"/>
       <c r="C19" s="41"/>
@@ -2424,7 +2427,7 @@
       <c r="K19" s="43"/>
       <c r="M19" s="52"/>
     </row>
-    <row r="20" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="e">
         <f>'1.Estimate'!#REF!</f>
         <v>#REF!</v>
@@ -2471,7 +2474,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
       <c r="B21" s="48" t="e">
         <f>'1.Estimate'!#REF!</f>
@@ -2500,7 +2503,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="22"/>
       <c r="C22" s="41"/>
@@ -2514,7 +2517,7 @@
       <c r="K22" s="43"/>
       <c r="M22" s="52"/>
     </row>
-    <row r="23" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="49">
         <f>'1.Estimate'!A17</f>
         <v>3</v>
@@ -2561,7 +2564,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="48" t="str">
         <f>'1.Estimate'!B21</f>
@@ -2590,7 +2593,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="22"/>
       <c r="C25" s="41"/>
@@ -2604,7 +2607,7 @@
       <c r="K25" s="43"/>
       <c r="M25" s="52"/>
     </row>
-    <row r="26" spans="1:13" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="e">
         <f>'1.Estimate'!#REF!</f>
         <v>#REF!</v>
@@ -2651,7 +2654,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
       <c r="B27" s="48" t="e">
         <f>'1.Estimate'!#REF!</f>
@@ -2680,7 +2683,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="22"/>
       <c r="C28" s="41"/>
@@ -2694,7 +2697,7 @@
       <c r="K28" s="43"/>
       <c r="M28" s="52"/>
     </row>
-    <row r="29" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49">
         <f>'1.Estimate'!A25</f>
         <v>5</v>
@@ -2741,7 +2744,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
       <c r="B30" s="22"/>
       <c r="C30" s="41"/>
@@ -2754,7 +2757,7 @@
       <c r="J30" s="42"/>
       <c r="K30" s="43"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="45" t="s">
         <v>42</v>
@@ -2778,7 +2781,7 @@
       </c>
       <c r="K31" s="23"/>
     </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K36">
         <v>1070</v>
       </c>
@@ -2830,25 +2833,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +2866,7 @@
       <c r="J1" s="63"/>
       <c r="K1" s="63"/>
     </row>
-    <row r="2" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>1</v>
       </c>
@@ -2878,7 +2881,7 @@
       <c r="J2" s="64"/>
       <c r="K2" s="64"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
@@ -2893,7 +2896,7 @@
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
@@ -2908,7 +2911,7 @@
       <c r="J4" s="65"/>
       <c r="K4" s="65"/>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>4</v>
       </c>
@@ -2923,9 +2926,9 @@
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="61" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B6" s="61"/>
       <c r="C6" s="61"/>
@@ -2940,7 +2943,7 @@
       <c r="J6" s="62"/>
       <c r="K6" s="62"/>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>6</v>
       </c>
@@ -2957,7 +2960,7 @@
       <c r="J7" s="69"/>
       <c r="K7" s="69"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2992,7 +2995,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -3009,14 +3012,14 @@
       <c r="J9" s="15"/>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="17">
         <v>0.5</v>
       </c>
       <c r="D10" s="18">
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="E10" s="18">
         <v>0.82</v>
@@ -3026,14 +3029,14 @@
       </c>
       <c r="G10" s="19">
         <f>(PRODUCT(C10:F10))</f>
-        <v>14.35</v>
+        <v>13.53</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
         <v>18</v>
@@ -3044,7 +3047,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="13">
         <f>SUM(G10:G10)</f>
-        <v>14.35</v>
+        <v>13.53</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>19</v>
@@ -3054,11 +3057,11 @@
       </c>
       <c r="J11" s="15">
         <f>G11*I11</f>
-        <v>9518.4984999999997</v>
+        <v>8974.5842999999986</v>
       </c>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
@@ -3071,7 +3074,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
@@ -3084,7 +3087,7 @@
       <c r="J13" s="15"/>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>2</v>
       </c>
@@ -3101,7 +3104,7 @@
       <c r="J14" s="15"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="9" t="s">
         <v>56</v>
@@ -3112,18 +3115,18 @@
       </c>
       <c r="D15" s="11">
         <f>D10</f>
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="E15" s="12">
         <v>0.38</v>
       </c>
       <c r="F15" s="18">
         <f>ROUNDUP(D15/E15,0)</f>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G15" s="19">
         <f>F15*C15</f>
-        <v>705</v>
+        <v>660</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="13"/>
@@ -3132,7 +3135,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
         <v>18</v>
@@ -3143,7 +3146,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="13">
         <f>SUM(G15:G15)</f>
-        <v>705</v>
+        <v>660</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>49</v>
@@ -3153,11 +3156,11 @@
       </c>
       <c r="J16" s="15">
         <f>G16*I16</f>
-        <v>64860</v>
+        <v>60720</v>
       </c>
       <c r="K16" s="72"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
@@ -3170,7 +3173,7 @@
       <c r="J17" s="15"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>3</v>
       </c>
@@ -3187,7 +3190,7 @@
       <c r="J18" s="15"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
         <v>47</v>
@@ -3210,7 +3213,7 @@
       <c r="J19" s="20"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
         <v>48</v>
@@ -3220,20 +3223,20 @@
       </c>
       <c r="D20" s="18">
         <f>D15</f>
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="19">
         <f>PRODUCT(C20:F20)</f>
-        <v>87.5</v>
+        <v>82.5</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
         <v>18</v>
@@ -3244,7 +3247,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="13">
         <f>(SUM(G19:G20))/6</f>
-        <v>22.583333333333332</v>
+        <v>21.75</v>
       </c>
       <c r="H21" s="14" t="s">
         <v>9</v>
@@ -3254,11 +3257,11 @@
       </c>
       <c r="J21" s="15">
         <f>G21*I21</f>
-        <v>5420</v>
+        <v>5220</v>
       </c>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
         <v>20</v>
@@ -3272,11 +3275,11 @@
       <c r="I22" s="13"/>
       <c r="J22" s="15">
         <f>0.13*J21</f>
-        <v>704.6</v>
+        <v>678.6</v>
       </c>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -3289,7 +3292,7 @@
       <c r="J23" s="15"/>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>4</v>
       </c>
@@ -3318,7 +3321,7 @@
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
@@ -3331,7 +3334,7 @@
       <c r="J25" s="15"/>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>5</v>
       </c>
@@ -3360,7 +3363,7 @@
       </c>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="24"/>
       <c r="C27" s="10"/>
@@ -3373,7 +3376,7 @@
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="35" t="s">
         <v>29</v>
@@ -3387,11 +3390,11 @@
       <c r="I28" s="15"/>
       <c r="J28" s="15">
         <f>SUM(J9:J26)</f>
-        <v>84003.098500000007</v>
+        <v>79093.184300000008</v>
       </c>
       <c r="K28" s="17"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="53"/>
       <c r="B29" s="54"/>
       <c r="C29" s="55"/>
@@ -3404,14 +3407,14 @@
       <c r="J29" s="57"/>
       <c r="K29" s="58"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="67">
         <f>J28</f>
-        <v>84003.098500000007</v>
+        <v>79093.184300000008</v>
       </c>
       <c r="D30" s="67"/>
       <c r="E30" s="19">
@@ -3424,13 +3427,13 @@
       <c r="J30" s="30"/>
       <c r="K30" s="31"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
       <c r="B31" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="70">
-        <v>75000</v>
+        <v>70000</v>
       </c>
       <c r="D31" s="70"/>
       <c r="E31" s="19"/>
@@ -3441,19 +3444,19 @@
       <c r="J31" s="34"/>
       <c r="K31" s="33"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="32"/>
       <c r="B32" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="70">
         <f>C31-C34-C35</f>
-        <v>71250</v>
+        <v>66500</v>
       </c>
       <c r="D32" s="70"/>
       <c r="E32" s="19">
         <f>C32/C30*100</f>
-        <v>84.818299886878563</v>
+        <v>84.078041096140311</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32" s="34"/>
@@ -3462,19 +3465,19 @@
       <c r="J32" s="34"/>
       <c r="K32" s="33"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="22" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="67">
         <f>C30-C32</f>
-        <v>12753.098500000007</v>
+        <v>12593.184300000008</v>
       </c>
       <c r="D33" s="67"/>
       <c r="E33" s="19">
         <f>100-E32</f>
-        <v>15.181700113121437</v>
+        <v>15.921958903859689</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="34"/>
@@ -3483,14 +3486,14 @@
       <c r="J33" s="34"/>
       <c r="K33" s="33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
       <c r="B34" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C34" s="67">
         <f>C31*0.03</f>
-        <v>2250</v>
+        <v>2100</v>
       </c>
       <c r="D34" s="67"/>
       <c r="E34" s="19">
@@ -3503,14 +3506,14 @@
       <c r="J34" s="34"/>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="32"/>
       <c r="B35" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="67">
         <f>C31*0.02</f>
-        <v>1500</v>
+        <v>1400</v>
       </c>
       <c r="D35" s="67"/>
       <c r="E35" s="19">
@@ -3534,13 +3537,13 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chinimaya mam pahiro samrakxan kaarya 200000
</commit_message>
<xml_diff>
--- a/ofc/estimates/Baniyaa gaun/chinimaya mam ghar paxadi.xlsx
+++ b/ofc/estimates/Baniyaa gaun/chinimaya mam ghar paxadi.xlsx
@@ -4,23 +4,25 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1.Estimate" sheetId="15" r:id="rId1"/>
     <sheet name="WCR" sheetId="7" r:id="rId2"/>
     <sheet name="2.Estimate" sheetId="18" r:id="rId3"/>
+    <sheet name="3.Estimate" sheetId="19" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
     <definedName name="description_124" localSheetId="2">#REF!</definedName>
+    <definedName name="description_124" localSheetId="3">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
     <definedName name="description_247">[1]Abstract!$B$22</definedName>
     <definedName name="description_248">[1]Abstract!$B$23</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="58">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -575,24 +577,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,6 +593,51 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -616,33 +645,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1306,113 +1308,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1569,7 +1571,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="13"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="71" t="s">
+      <c r="K14" s="65" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1596,7 +1598,7 @@
         <f>G15*I15</f>
         <v>18400</v>
       </c>
-      <c r="K15" s="72"/>
+      <c r="K15" s="66"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -1850,11 +1852,11 @@
       <c r="B29" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="67">
+      <c r="C29" s="61">
         <f>J27</f>
         <v>34748.313000000002</v>
       </c>
-      <c r="D29" s="67"/>
+      <c r="D29" s="61"/>
       <c r="E29" s="19">
         <v>100</v>
       </c>
@@ -1870,10 +1872,10 @@
       <c r="B30" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="70">
+      <c r="C30" s="64">
         <v>30000</v>
       </c>
-      <c r="D30" s="70"/>
+      <c r="D30" s="64"/>
       <c r="E30" s="19"/>
       <c r="F30" s="33"/>
       <c r="G30" s="34"/>
@@ -1887,11 +1889,11 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="70">
+      <c r="C31" s="64">
         <f>C30-C33-C34</f>
         <v>28500</v>
       </c>
-      <c r="D31" s="70"/>
+      <c r="D31" s="64"/>
       <c r="E31" s="19">
         <f>C31/C29*100</f>
         <v>82.018370215555493</v>
@@ -1908,11 +1910,11 @@
       <c r="B32" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="67">
+      <c r="C32" s="61">
         <f>C29-C31</f>
         <v>6248.3130000000019</v>
       </c>
-      <c r="D32" s="67"/>
+      <c r="D32" s="61"/>
       <c r="E32" s="19">
         <f>100-E31</f>
         <v>17.981629784444507</v>
@@ -1929,11 +1931,11 @@
       <c r="B33" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="67">
+      <c r="C33" s="61">
         <f>C30*0.03</f>
         <v>900</v>
       </c>
-      <c r="D33" s="67"/>
+      <c r="D33" s="61"/>
       <c r="E33" s="19">
         <v>3</v>
       </c>
@@ -1949,11 +1951,11 @@
       <c r="B34" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="67">
+      <c r="C34" s="61">
         <f>C30*0.02</f>
         <v>600</v>
       </c>
-      <c r="D34" s="67"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="19">
         <v>2</v>
       </c>
@@ -1966,6 +1968,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="A7:F7"/>
@@ -1975,13 +1984,6 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="K14:K15"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2019,90 +2021,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
     </row>
     <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
     </row>
     <row r="4" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="37"/>
-      <c r="C6" s="80" t="e">
+      <c r="C6" s="73" t="e">
         <f>F31</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="81"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="38"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
@@ -2110,11 +2112,11 @@
         <v>32</v>
       </c>
       <c r="I6" s="37"/>
-      <c r="J6" s="80" t="e">
+      <c r="J6" s="73" t="e">
         <f>I31</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="81"/>
+      <c r="K6" s="74"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
@@ -2123,77 +2125,77 @@
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="I7" s="77" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="e">
+      <c r="A8" s="67" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="I8" s="78" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="I8" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="e">
+      <c r="A9" s="81" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="I9" s="78" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="I9" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75" t="s">
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="74" t="s">
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="73" t="s">
+      <c r="K11" s="82" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="40" t="s">
         <v>41</v>
       </c>
@@ -2212,8 +2214,8 @@
       <c r="I12" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="73"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="82"/>
     </row>
     <row r="13" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49" t="e">
@@ -2796,6 +2798,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2803,19 +2818,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2833,7 +2835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:K5"/>
     </sheetView>
   </sheetViews>
@@ -2852,113 +2854,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -3131,7 +3133,7 @@
       <c r="H15" s="14"/>
       <c r="I15" s="13"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="71" t="s">
+      <c r="K15" s="65" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3158,7 +3160,7 @@
         <f>G16*I16</f>
         <v>60720</v>
       </c>
-      <c r="K16" s="72"/>
+      <c r="K16" s="66"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
@@ -3412,11 +3414,11 @@
       <c r="B30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="67">
+      <c r="C30" s="61">
         <f>J28</f>
         <v>79093.184300000008</v>
       </c>
-      <c r="D30" s="67"/>
+      <c r="D30" s="61"/>
       <c r="E30" s="19">
         <v>100</v>
       </c>
@@ -3432,10 +3434,10 @@
       <c r="B31" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="70">
+      <c r="C31" s="64">
         <v>70000</v>
       </c>
-      <c r="D31" s="70"/>
+      <c r="D31" s="64"/>
       <c r="E31" s="19"/>
       <c r="F31" s="33"/>
       <c r="G31" s="34"/>
@@ -3449,11 +3451,11 @@
       <c r="B32" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="70">
+      <c r="C32" s="64">
         <f>C31-C34-C35</f>
         <v>66500</v>
       </c>
-      <c r="D32" s="70"/>
+      <c r="D32" s="64"/>
       <c r="E32" s="19">
         <f>C32/C30*100</f>
         <v>84.078041096140311</v>
@@ -3470,11 +3472,11 @@
       <c r="B33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="67">
+      <c r="C33" s="61">
         <f>C30-C32</f>
         <v>12593.184300000008</v>
       </c>
-      <c r="D33" s="67"/>
+      <c r="D33" s="61"/>
       <c r="E33" s="19">
         <f>100-E32</f>
         <v>15.921958903859689</v>
@@ -3491,11 +3493,11 @@
       <c r="B34" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="67">
+      <c r="C34" s="61">
         <f>C31*0.03</f>
         <v>2100</v>
       </c>
-      <c r="D34" s="67"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="19">
         <v>3</v>
       </c>
@@ -3511,11 +3513,742 @@
       <c r="B35" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="67">
+      <c r="C35" s="61">
         <f>C31*0.02</f>
         <v>1400</v>
       </c>
-      <c r="D35" s="67"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="19">
+        <v>2</v>
+      </c>
+      <c r="F35" s="33"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+    </row>
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="17">
+        <f>2*0.5</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="18">
+        <f>24</f>
+        <v>24</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.82</v>
+      </c>
+      <c r="F10" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="G10" s="19">
+        <f>(PRODUCT(C10:F10))</f>
+        <v>31.488</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13">
+        <f>SUM(G10:G10)</f>
+        <v>31.488</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="13">
+        <v>663.31</v>
+      </c>
+      <c r="J11" s="15">
+        <f>G11*I11</f>
+        <v>20886.305279999997</v>
+      </c>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="10">
+        <f>2*(3*5)</f>
+        <v>30</v>
+      </c>
+      <c r="D15" s="11">
+        <f>D10</f>
+        <v>24</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="F15" s="18">
+        <f>ROUNDUP(D15/E15,0)</f>
+        <v>64</v>
+      </c>
+      <c r="G15" s="19">
+        <f>F15*C15</f>
+        <v>1920</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13">
+        <f>SUM(G15:G15)</f>
+        <v>1920</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="13">
+        <v>92</v>
+      </c>
+      <c r="J16" s="15">
+        <f>G16*I16</f>
+        <v>176640</v>
+      </c>
+      <c r="K16" s="66"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="36">
+        <f>2*(TRUNC(D15/1.5,0)+1)</f>
+        <v>34</v>
+      </c>
+      <c r="D19" s="18">
+        <v>4</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19">
+        <f>PRODUCT(C19:F19)</f>
+        <v>136</v>
+      </c>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="36">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D20" s="18">
+        <f>D15</f>
+        <v>24</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19">
+        <f>PRODUCT(C20:F20)</f>
+        <v>240</v>
+      </c>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13">
+        <f>TRUNC((SUM(G19:G20))/6,0)+1</f>
+        <v>63</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="13">
+        <v>240</v>
+      </c>
+      <c r="J21" s="15">
+        <f>G21*I21</f>
+        <v>15120</v>
+      </c>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="15">
+        <f>0.13*J21</f>
+        <v>1965.6000000000001</v>
+      </c>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>4</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="25">
+        <f t="shared" ref="G24" si="0">PRODUCT(C24:F24)</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="13">
+        <f>G16*5</f>
+        <v>9600</v>
+      </c>
+      <c r="J24" s="25">
+        <f>G24*I24</f>
+        <v>9600</v>
+      </c>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="25">
+        <f t="shared" ref="G26" si="1">PRODUCT(C26:F26)</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="13">
+        <v>500</v>
+      </c>
+      <c r="J26" s="25">
+        <f>G26*I26</f>
+        <v>500</v>
+      </c>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="36"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15">
+        <f>SUM(J9:J26)</f>
+        <v>224711.90528000001</v>
+      </c>
+      <c r="K28" s="17"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="58"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="61">
+        <f>J28</f>
+        <v>224711.90528000001</v>
+      </c>
+      <c r="D30" s="61"/>
+      <c r="E30" s="19">
+        <v>100</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="64">
+        <v>200000</v>
+      </c>
+      <c r="D31" s="64"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="33"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="64">
+        <f>C31-C34-C35</f>
+        <v>190000</v>
+      </c>
+      <c r="D32" s="64"/>
+      <c r="E32" s="19">
+        <f>C32/C30*100</f>
+        <v>84.552707504861573</v>
+      </c>
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="33"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="61">
+        <f>C30-C32</f>
+        <v>34711.905280000006</v>
+      </c>
+      <c r="D33" s="61"/>
+      <c r="E33" s="19">
+        <f>100-E32</f>
+        <v>15.447292495138427</v>
+      </c>
+      <c r="F33" s="33"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="33"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="61">
+        <f>C31*0.03</f>
+        <v>6000</v>
+      </c>
+      <c r="D34" s="61"/>
+      <c r="E34" s="19">
+        <v>3</v>
+      </c>
+      <c r="F34" s="33"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="33"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="61">
+        <f>C31*0.02</f>
+        <v>4000</v>
+      </c>
+      <c r="D35" s="61"/>
       <c r="E35" s="19">
         <v>2</v>
       </c>
@@ -3537,13 +4270,13 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
name change of upabhokta for chinimaya mam
</commit_message>
<xml_diff>
--- a/ofc/estimates/Baniyaa gaun/chinimaya mam ghar paxadi.xlsx
+++ b/ofc/estimates/Baniyaa gaun/chinimaya mam ghar paxadi.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="59">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">Project:- मनोहरा नदि कटानबाट पहिरो संरक्षण कार्य </t>
+  </si>
+  <si>
+    <t>Project:- कुसुमथली पहिरो संरक्षण</t>
   </si>
 </sst>
 </file>
@@ -577,6 +580,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -593,23 +614,26 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,27 +648,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1308,113 +1311,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1571,7 +1574,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="13"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="65" t="s">
+      <c r="K14" s="71" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1598,7 +1601,7 @@
         <f>G15*I15</f>
         <v>18400</v>
       </c>
-      <c r="K15" s="66"/>
+      <c r="K15" s="72"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -1852,11 +1855,11 @@
       <c r="B29" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="61">
+      <c r="C29" s="67">
         <f>J27</f>
         <v>34748.313000000002</v>
       </c>
-      <c r="D29" s="61"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="19">
         <v>100</v>
       </c>
@@ -1872,10 +1875,10 @@
       <c r="B30" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="64">
+      <c r="C30" s="70">
         <v>30000</v>
       </c>
-      <c r="D30" s="64"/>
+      <c r="D30" s="70"/>
       <c r="E30" s="19"/>
       <c r="F30" s="33"/>
       <c r="G30" s="34"/>
@@ -1889,11 +1892,11 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="64">
+      <c r="C31" s="70">
         <f>C30-C33-C34</f>
         <v>28500</v>
       </c>
-      <c r="D31" s="64"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="19">
         <f>C31/C29*100</f>
         <v>82.018370215555493</v>
@@ -1910,11 +1913,11 @@
       <c r="B32" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="61">
+      <c r="C32" s="67">
         <f>C29-C31</f>
         <v>6248.3130000000019</v>
       </c>
-      <c r="D32" s="61"/>
+      <c r="D32" s="67"/>
       <c r="E32" s="19">
         <f>100-E31</f>
         <v>17.981629784444507</v>
@@ -1931,11 +1934,11 @@
       <c r="B33" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="61">
+      <c r="C33" s="67">
         <f>C30*0.03</f>
         <v>900</v>
       </c>
-      <c r="D33" s="61"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="19">
         <v>3</v>
       </c>
@@ -1951,11 +1954,11 @@
       <c r="B34" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="61">
+      <c r="C34" s="67">
         <f>C30*0.02</f>
         <v>600</v>
       </c>
-      <c r="D34" s="61"/>
+      <c r="D34" s="67"/>
       <c r="E34" s="19">
         <v>2</v>
       </c>
@@ -1968,13 +1971,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="A7:F7"/>
@@ -1984,6 +1980,13 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="K14:K15"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2021,90 +2024,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
     </row>
     <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="37"/>
-      <c r="C6" s="73" t="e">
+      <c r="C6" s="80" t="e">
         <f>F31</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="74"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="38"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
@@ -2112,11 +2115,11 @@
         <v>32</v>
       </c>
       <c r="I6" s="37"/>
-      <c r="J6" s="73" t="e">
+      <c r="J6" s="80" t="e">
         <f>I31</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="74"/>
+      <c r="K6" s="81"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
@@ -2125,77 +2128,77 @@
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="I7" s="79" t="s">
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="I7" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="e">
+      <c r="A8" s="61" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="I8" s="80" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="I8" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="e">
+      <c r="A9" s="79" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="I9" s="80" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="I9" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84" t="s">
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="83" t="s">
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="82" t="s">
+      <c r="K11" s="73" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="40" t="s">
         <v>41</v>
       </c>
@@ -2214,8 +2217,8 @@
       <c r="I12" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="83"/>
-      <c r="K12" s="82"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="73"/>
     </row>
     <row r="13" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49" t="e">
@@ -2798,6 +2801,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
@@ -2805,19 +2821,6 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2854,113 +2857,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -3133,7 +3136,7 @@
       <c r="H15" s="14"/>
       <c r="I15" s="13"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="65" t="s">
+      <c r="K15" s="71" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3160,7 +3163,7 @@
         <f>G16*I16</f>
         <v>60720</v>
       </c>
-      <c r="K16" s="66"/>
+      <c r="K16" s="72"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
@@ -3414,11 +3417,11 @@
       <c r="B30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="61">
+      <c r="C30" s="67">
         <f>J28</f>
         <v>79093.184300000008</v>
       </c>
-      <c r="D30" s="61"/>
+      <c r="D30" s="67"/>
       <c r="E30" s="19">
         <v>100</v>
       </c>
@@ -3434,10 +3437,10 @@
       <c r="B31" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="64">
+      <c r="C31" s="70">
         <v>70000</v>
       </c>
-      <c r="D31" s="64"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="19"/>
       <c r="F31" s="33"/>
       <c r="G31" s="34"/>
@@ -3451,11 +3454,11 @@
       <c r="B32" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="64">
+      <c r="C32" s="70">
         <f>C31-C34-C35</f>
         <v>66500</v>
       </c>
-      <c r="D32" s="64"/>
+      <c r="D32" s="70"/>
       <c r="E32" s="19">
         <f>C32/C30*100</f>
         <v>84.078041096140311</v>
@@ -3472,11 +3475,11 @@
       <c r="B33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="61">
+      <c r="C33" s="67">
         <f>C30-C32</f>
         <v>12593.184300000008</v>
       </c>
-      <c r="D33" s="61"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="19">
         <f>100-E32</f>
         <v>15.921958903859689</v>
@@ -3493,11 +3496,11 @@
       <c r="B34" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="61">
+      <c r="C34" s="67">
         <f>C31*0.03</f>
         <v>2100</v>
       </c>
-      <c r="D34" s="61"/>
+      <c r="D34" s="67"/>
       <c r="E34" s="19">
         <v>3</v>
       </c>
@@ -3513,11 +3516,742 @@
       <c r="B35" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="61">
+      <c r="C35" s="67">
         <f>C31*0.02</f>
         <v>1400</v>
       </c>
-      <c r="D35" s="61"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="19">
+        <v>2</v>
+      </c>
+      <c r="F35" s="33"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+    </row>
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="17">
+        <f>2*0.5</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="18">
+        <f>24</f>
+        <v>24</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.82</v>
+      </c>
+      <c r="F10" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="G10" s="19">
+        <f>(PRODUCT(C10:F10))</f>
+        <v>31.488</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13">
+        <f>SUM(G10:G10)</f>
+        <v>31.488</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="13">
+        <v>663.31</v>
+      </c>
+      <c r="J11" s="15">
+        <f>G11*I11</f>
+        <v>20886.305279999997</v>
+      </c>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="10">
+        <f>2*(3*5)</f>
+        <v>30</v>
+      </c>
+      <c r="D15" s="11">
+        <f>D10</f>
+        <v>24</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="F15" s="18">
+        <f>ROUNDUP(D15/E15,0)</f>
+        <v>64</v>
+      </c>
+      <c r="G15" s="19">
+        <f>F15*C15</f>
+        <v>1920</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="71" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13">
+        <f>SUM(G15:G15)</f>
+        <v>1920</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="13">
+        <v>92</v>
+      </c>
+      <c r="J16" s="15">
+        <f>G16*I16</f>
+        <v>176640</v>
+      </c>
+      <c r="K16" s="72"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>3</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="36">
+        <f>2*(TRUNC(D15/1.5,0)+1)</f>
+        <v>34</v>
+      </c>
+      <c r="D19" s="18">
+        <v>4</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19">
+        <f>PRODUCT(C19:F19)</f>
+        <v>136</v>
+      </c>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="36">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D20" s="18">
+        <f>D15</f>
+        <v>24</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19">
+        <f>PRODUCT(C20:F20)</f>
+        <v>240</v>
+      </c>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13">
+        <f>TRUNC((SUM(G19:G20))/6,0)+1</f>
+        <v>63</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="13">
+        <v>240</v>
+      </c>
+      <c r="J21" s="15">
+        <f>G21*I21</f>
+        <v>15120</v>
+      </c>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="15">
+        <f>0.13*J21</f>
+        <v>1965.6000000000001</v>
+      </c>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>4</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="25">
+        <f t="shared" ref="G24" si="0">PRODUCT(C24:F24)</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="13">
+        <f>G16*5</f>
+        <v>9600</v>
+      </c>
+      <c r="J24" s="25">
+        <f>G24*I24</f>
+        <v>9600</v>
+      </c>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="25">
+        <f t="shared" ref="G26" si="1">PRODUCT(C26:F26)</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="13">
+        <v>500</v>
+      </c>
+      <c r="J26" s="25">
+        <f>G26*I26</f>
+        <v>500</v>
+      </c>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="36"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15">
+        <f>SUM(J9:J26)</f>
+        <v>224711.90528000001</v>
+      </c>
+      <c r="K28" s="17"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="58"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="67">
+        <f>J28</f>
+        <v>224711.90528000001</v>
+      </c>
+      <c r="D30" s="67"/>
+      <c r="E30" s="19">
+        <v>100</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="70">
+        <v>200000</v>
+      </c>
+      <c r="D31" s="70"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="33"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="70">
+        <f>C31-C34-C35</f>
+        <v>190000</v>
+      </c>
+      <c r="D32" s="70"/>
+      <c r="E32" s="19">
+        <f>C32/C30*100</f>
+        <v>84.552707504861573</v>
+      </c>
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="33"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="67">
+        <f>C30-C32</f>
+        <v>34711.905280000006</v>
+      </c>
+      <c r="D33" s="67"/>
+      <c r="E33" s="19">
+        <f>100-E32</f>
+        <v>15.447292495138427</v>
+      </c>
+      <c r="F33" s="33"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="33"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="67">
+        <f>C31*0.03</f>
+        <v>6000</v>
+      </c>
+      <c r="D34" s="67"/>
+      <c r="E34" s="19">
+        <v>3</v>
+      </c>
+      <c r="F34" s="33"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="33"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="67">
+        <f>C31*0.02</f>
+        <v>4000</v>
+      </c>
+      <c r="D35" s="67"/>
       <c r="E35" s="19">
         <v>2</v>
       </c>
@@ -3556,735 +4290,4 @@
 </oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-    </row>
-    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="68" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>1</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="17">
-        <f>2*0.5</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="18">
-        <f>24</f>
-        <v>24</v>
-      </c>
-      <c r="E10" s="18">
-        <v>0.82</v>
-      </c>
-      <c r="F10" s="18">
-        <v>1.6</v>
-      </c>
-      <c r="G10" s="19">
-        <f>(PRODUCT(C10:F10))</f>
-        <v>31.488</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13">
-        <f>SUM(G10:G10)</f>
-        <v>31.488</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="13">
-        <v>663.31</v>
-      </c>
-      <c r="J11" s="15">
-        <f>G11*I11</f>
-        <v>20886.305279999997</v>
-      </c>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="10">
-        <f>2*(3*5)</f>
-        <v>30</v>
-      </c>
-      <c r="D15" s="11">
-        <f>D10</f>
-        <v>24</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0.38</v>
-      </c>
-      <c r="F15" s="18">
-        <f>ROUNDUP(D15/E15,0)</f>
-        <v>64</v>
-      </c>
-      <c r="G15" s="19">
-        <f>F15*C15</f>
-        <v>1920</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="65" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13">
-        <f>SUM(G15:G15)</f>
-        <v>1920</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="13">
-        <v>92</v>
-      </c>
-      <c r="J16" s="15">
-        <f>G16*I16</f>
-        <v>176640</v>
-      </c>
-      <c r="K16" s="66"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>3</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="36">
-        <f>2*(TRUNC(D15/1.5,0)+1)</f>
-        <v>34</v>
-      </c>
-      <c r="D19" s="18">
-        <v>4</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19">
-        <f>PRODUCT(C19:F19)</f>
-        <v>136</v>
-      </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="36">
-        <f>2*5</f>
-        <v>10</v>
-      </c>
-      <c r="D20" s="18">
-        <f>D15</f>
-        <v>24</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19">
-        <f>PRODUCT(C20:F20)</f>
-        <v>240</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13">
-        <f>TRUNC((SUM(G19:G20))/6,0)+1</f>
-        <v>63</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="13">
-        <v>240</v>
-      </c>
-      <c r="J21" s="15">
-        <f>G21*I21</f>
-        <v>15120</v>
-      </c>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="15">
-        <f>0.13*J21</f>
-        <v>1965.6000000000001</v>
-      </c>
-      <c r="K22" s="12"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>4</v>
-      </c>
-      <c r="B24" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="10">
-        <v>1</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="25">
-        <f t="shared" ref="G24" si="0">PRODUCT(C24:F24)</f>
-        <v>1</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="13">
-        <f>G16*5</f>
-        <v>9600</v>
-      </c>
-      <c r="J24" s="25">
-        <f>G24*I24</f>
-        <v>9600</v>
-      </c>
-      <c r="K24" s="12"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="12"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>5</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="10">
-        <v>1</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="25">
-        <f t="shared" ref="G26" si="1">PRODUCT(C26:F26)</f>
-        <v>1</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="13">
-        <v>500</v>
-      </c>
-      <c r="J26" s="25">
-        <f>G26*I26</f>
-        <v>500</v>
-      </c>
-      <c r="K26" s="12"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="12"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15">
-        <f>SUM(J9:J26)</f>
-        <v>224711.90528000001</v>
-      </c>
-      <c r="K28" s="17"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="58"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="61">
-        <f>J28</f>
-        <v>224711.90528000001</v>
-      </c>
-      <c r="D30" s="61"/>
-      <c r="E30" s="19">
-        <v>100</v>
-      </c>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="31"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="64">
-        <v>200000</v>
-      </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="33"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="64">
-        <f>C31-C34-C35</f>
-        <v>190000</v>
-      </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="19">
-        <f>C32/C30*100</f>
-        <v>84.552707504861573</v>
-      </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="33"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="61">
-        <f>C30-C32</f>
-        <v>34711.905280000006</v>
-      </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="19">
-        <f>100-E32</f>
-        <v>15.447292495138427</v>
-      </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="33"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="61">
-        <f>C31*0.03</f>
-        <v>6000</v>
-      </c>
-      <c r="D34" s="61"/>
-      <c r="E34" s="19">
-        <v>3</v>
-      </c>
-      <c r="F34" s="33"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="33"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="61">
-        <f>C31*0.02</f>
-        <v>4000</v>
-      </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="19">
-        <v>2</v>
-      </c>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="33"/>
-    </row>
-  </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter xml:space="preserve">&amp;LPrepared By:
-&amp;CChecked By:
-&amp;RApproved By:
-</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>